<commit_message>
Updated pmfs and stats data.
</commit_message>
<xml_diff>
--- a/data/absorption_time_stats.xlsx
+++ b/data/absorption_time_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,14 +453,18 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>model_pve_border</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.5131086142322095</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.4868913857677895</v>
+          <t>amc_pve_border</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>71.11610486891385</v>
@@ -469,369 +473,669 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>model_pve_center</t>
+          <t>model_pve_border</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3049242424242409</v>
+        <v>0.5131086142322095</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6950757575757576</v>
+        <v>0.4868913857677895</v>
       </c>
       <c r="D3" t="n">
-        <v>145.4488636363634</v>
+        <v>71.11610486891385</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>model_bvb</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.4957689733196263</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.5042310266803719</v>
+          <t>amc_pve_center</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D4" t="n">
-        <v>75.2084649768138</v>
+        <v>145.4488636363635</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>model_pve_border_pure</t>
+          <t>model_pve_center</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5122443535433675</v>
+        <v>0.3049242424242409</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4877556464566302</v>
+        <v>0.6950757575757576</v>
       </c>
       <c r="D5" t="n">
-        <v>73.7926856681966</v>
+        <v>145.4488636363634</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>model_pve_center_pure</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.3035013989275322</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.6964986010724641</v>
+          <t>amc_bvb</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D6" t="n">
-        <v>145.8494291697252</v>
+        <v>75.20846497681381</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>model_pvp</t>
+          <t>model_bvb</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3527054108216414</v>
+        <v>0.4957689733196263</v>
       </c>
       <c r="C7" t="n">
-        <v>0.647294589178356</v>
+        <v>0.5042310266803719</v>
       </c>
       <c r="D7" t="n">
-        <v>120.5991983967936</v>
+        <v>75.2084649768138</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>model_pvp_pure</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.3634039729644691</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.6365960270355299</v>
+          <t>amc_pve_border_pure</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D8" t="n">
-        <v>116.2167676623678</v>
+        <v>73.79268566819664</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>model_pvp_400</t>
+          <t>model_pve_border_pure</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.153846151305991</v>
+        <v>0.5122443535433675</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8461538323247217</v>
+        <v>0.4877556464566302</v>
       </c>
       <c r="D9" t="n">
-        <v>597.6152118280573</v>
+        <v>73.7926856681966</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>model_pvp_400_pure</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.3139555516908658</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.68604444830913</v>
+          <t>amc_pve_center_pure</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D10" t="n">
-        <v>133.2213405843279</v>
+        <v>145.8494291697253</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>model_pve_border_optimal</t>
+          <t>model_pve_center_pure</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9999999999999986</v>
+        <v>0.3035013989275322</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.6964986010724641</v>
       </c>
       <c r="D11" t="n">
-        <v>64.00000000000001</v>
+        <v>145.8494291697252</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>model_pve_center_optimal</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.9999999999999922</v>
+          <t>amc_pvp</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D12" t="n">
-        <v>224.9999999999999</v>
+        <v>120.5991983967938</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>model_pve_center_optimal_2d</t>
+          <t>model_pvp</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>0.3527054108216414</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9999999999999923</v>
+        <v>0.647294589178356</v>
       </c>
       <c r="D13" t="n">
-        <v>224.9999999999999</v>
+        <v>120.5991983967936</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>simulation_pve_border</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0.5125</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.4875</v>
+          <t>amc_pvp_pure</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D14" t="n">
-        <v>71.3754</v>
+        <v>116.2167676623677</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>simulation_pve_center</t>
+          <t>model_pvp_pure</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.30333</v>
+        <v>0.3634039729644691</v>
       </c>
       <c r="C15" t="n">
-        <v>0.69667</v>
+        <v>0.6365960270355299</v>
       </c>
       <c r="D15" t="n">
-        <v>145.21339</v>
+        <v>116.2167676623678</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>simulation_bvb</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.49573</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.50427</v>
+          <t>amc_pvp_400</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D16" t="n">
-        <v>75.21819000000001</v>
+        <v>597.6153846153867</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>simulation_pve_border_pure</t>
+          <t>model_pvp_400</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.51309</v>
+        <v>0.153846151305991</v>
       </c>
       <c r="C17" t="n">
-        <v>0.48691</v>
+        <v>0.8461538323247217</v>
       </c>
       <c r="D17" t="n">
-        <v>73.66419</v>
+        <v>597.6152118280573</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>simulation_pve_center_pure</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>0.3018999999999999</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.6981000000000001</v>
+          <t>amc_pvp_400_pure</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D18" t="n">
-        <v>145.77444</v>
+        <v>133.2213405843278</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>simulation_pvp</t>
+          <t>model_pvp_400_pure</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.35157</v>
+        <v>0.3139555516908658</v>
       </c>
       <c r="C19" t="n">
-        <v>0.64843</v>
+        <v>0.68604444830913</v>
       </c>
       <c r="D19" t="n">
-        <v>120.90991</v>
+        <v>133.2213405843279</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>simulation_pvp_pure</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0.36382</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.63618</v>
+          <t>amc_pve_border_optimal</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D20" t="n">
-        <v>115.93462</v>
+        <v>63.99999999999999</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>simulation_pvp_400</t>
+          <t>model_pve_border_optimal</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.15518</v>
+        <v>0.9999999999999986</v>
       </c>
       <c r="C21" t="n">
-        <v>0.84482</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>594.2682600000001</v>
+        <v>64.00000000000001</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>simulation_pvp_400_pure</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.3152</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.6848</v>
+          <t>amc_pve_center_optimal</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D22" t="n">
-        <v>132.90866</v>
+        <v>224.9999999999992</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>simulation_pve_border_optimal</t>
+          <t>model_pve_center_optimal</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>0.9999999999999922</v>
       </c>
       <c r="D23" t="n">
-        <v>64.09062</v>
+        <v>224.9999999999999</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>simulation_pve_center_optimal</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1</v>
+          <t>amc_pve_center_optimal_2d</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
       </c>
       <c r="D24" t="n">
-        <v>224.34096</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>simulation_pve_center_optimal_2d</t>
+          <t>model_pve_center_optimal_2d</t>
         </is>
       </c>
       <c r="B25" t="n">
         <v>0</v>
       </c>
       <c r="C25" t="n">
+        <v>0.9999999999999923</v>
+      </c>
+      <c r="D25" t="n">
+        <v>224.9999999999999</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>experiment_pvp</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.3527054108216432</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.6472945891783568</v>
+      </c>
+      <c r="D26" t="n">
+        <v>120.5991983967936</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>experiment_pvp_400</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.8461538461538461</v>
+      </c>
+      <c r="D27" t="n">
+        <v>597.6153846153846</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>experiment_pve_border</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.5131086142322098</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.4868913857677902</v>
+      </c>
+      <c r="D28" t="n">
+        <v>71.11610486891385</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>experiment_pve_center</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.3049242424242424</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.6950757575757575</v>
+      </c>
+      <c r="D29" t="n">
+        <v>145.4488636363637</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pve_border</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.51451</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.48549</v>
+      </c>
+      <c r="D30" t="n">
+        <v>71.10605</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pve_center</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.30589</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.69411</v>
+      </c>
+      <c r="D31" t="n">
+        <v>145.03451</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>simulation_bvb</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.49629</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.50371</v>
+      </c>
+      <c r="D32" t="n">
+        <v>75.07893</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pve_border_pure</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.5137499999999999</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.48625</v>
+      </c>
+      <c r="D33" t="n">
+        <v>73.97411</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pve_center_pure</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.3051700000000001</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.6948299999999999</v>
+      </c>
+      <c r="D34" t="n">
+        <v>146.02841</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pvp</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.35373</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.64627</v>
+      </c>
+      <c r="D35" t="n">
+        <v>120.46097</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pvp_pure</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.36546</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.63454</v>
+      </c>
+      <c r="D36" t="n">
+        <v>116.63374</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pvp_400</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.15349</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.84651</v>
+      </c>
+      <c r="D37" t="n">
+        <v>596.75585</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pvp_400_pure</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.3146600000000001</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.6853399999999999</v>
+      </c>
+      <c r="D38" t="n">
+        <v>133.1163</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pve_border_optimal</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
         <v>1</v>
       </c>
-      <c r="D25" t="n">
-        <v>225.74888</v>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>64.22884000000001</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pve_center_optimal</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
+        <v>224.84414</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>simulation_pve_center_optimal_2d</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="n">
+        <v>225.78116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>